<commit_message>
created graph viz for Campus Crimes
</commit_message>
<xml_diff>
--- a/CampusCrimesMerged.xlsx
+++ b/CampusCrimesMerged.xlsx
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3466"/>
+  <dimension ref="A1:E3466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2725,7 +2725,7 @@
         <v>7288</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>6</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>7</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>8</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>9</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>11</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>12</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>13</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>5</v>
       </c>
@@ -2877,9 +2877,8 @@
       <c r="E137" s="1">
         <v>8405</v>
       </c>
-      <c r="F137" s="1"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>6</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>8</v>
       </c>
@@ -2930,7 +2929,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>9</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>10</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>11</v>
       </c>
@@ -2981,7 +2980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>12</v>
       </c>
@@ -4630,7 +4629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>10</v>
       </c>
@@ -4647,7 +4646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>11</v>
       </c>
@@ -4664,7 +4663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>12</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>13</v>
       </c>
@@ -4698,7 +4697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>5</v>
       </c>
@@ -4714,9 +4713,8 @@
       <c r="E245" s="1">
         <v>11144</v>
       </c>
-      <c r="F245" s="1"/>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>6</v>
       </c>
@@ -4733,7 +4731,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>7</v>
       </c>
@@ -4750,7 +4748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>8</v>
       </c>
@@ -4767,7 +4765,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>9</v>
       </c>
@@ -4784,7 +4782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>10</v>
       </c>
@@ -4801,7 +4799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>11</v>
       </c>
@@ -4818,7 +4816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>12</v>
       </c>
@@ -4835,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>13</v>
       </c>
@@ -4852,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>5</v>
       </c>
@@ -4869,7 +4867,7 @@
         <v>11017</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>6</v>
       </c>
@@ -4886,7 +4884,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>7</v>
       </c>
@@ -6535,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
         <v>5</v>
       </c>
@@ -6551,9 +6549,8 @@
       <c r="E353" s="1">
         <v>2</v>
       </c>
-      <c r="F353" s="1"/>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>6</v>
       </c>
@@ -6570,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
         <v>7</v>
       </c>
@@ -6587,7 +6584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>8</v>
       </c>
@@ -6604,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>9</v>
       </c>
@@ -6621,7 +6618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>10</v>
       </c>
@@ -6638,7 +6635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>11</v>
       </c>
@@ -6655,7 +6652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>12</v>
       </c>
@@ -6672,7 +6669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>13</v>
       </c>
@@ -6689,7 +6686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>5</v>
       </c>
@@ -6706,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
         <v>6</v>
       </c>
@@ -6723,7 +6720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>7</v>
       </c>
@@ -6740,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>8</v>
       </c>
@@ -6757,7 +6754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>9</v>
       </c>
@@ -6774,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>10</v>
       </c>
@@ -6791,7 +6788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>11</v>
       </c>
@@ -8168,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
         <v>11</v>
       </c>
@@ -8185,7 +8182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>12</v>
       </c>
@@ -8202,7 +8199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
         <v>13</v>
       </c>
@@ -8219,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>5</v>
       </c>
@@ -8236,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
         <v>6</v>
       </c>
@@ -8253,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>7</v>
       </c>
@@ -8270,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>8</v>
       </c>
@@ -8287,7 +8284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>9</v>
       </c>
@@ -8304,7 +8301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A457" s="1" t="s">
         <v>10</v>
       </c>
@@ -8321,7 +8318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>11</v>
       </c>
@@ -8338,7 +8335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
         <v>12</v>
       </c>
@@ -8355,7 +8352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
         <v>13</v>
       </c>
@@ -8372,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
         <v>5</v>
       </c>
@@ -8388,9 +8385,8 @@
       <c r="E461" s="1">
         <v>0</v>
       </c>
-      <c r="F461" s="1"/>
-    </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
         <v>6</v>
       </c>
@@ -8407,7 +8403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A463" s="1" t="s">
         <v>7</v>
       </c>
@@ -8424,7 +8420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
         <v>8</v>
       </c>
@@ -9801,7 +9797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="545" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A545" s="1" t="s">
         <v>8</v>
       </c>
@@ -9818,7 +9814,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="546" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A546" s="1" t="s">
         <v>9</v>
       </c>
@@ -9835,7 +9831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="547" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A547" s="1" t="s">
         <v>10</v>
       </c>
@@ -9852,7 +9848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="548" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A548" s="1" t="s">
         <v>11</v>
       </c>
@@ -9869,7 +9865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="549" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A549" s="1" t="s">
         <v>12</v>
       </c>
@@ -9886,7 +9882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="550" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A550" s="1" t="s">
         <v>13</v>
       </c>
@@ -9903,7 +9899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="551" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
         <v>5</v>
       </c>
@@ -9919,9 +9915,8 @@
       <c r="E551" s="1">
         <v>1653</v>
       </c>
-      <c r="F551" s="1"/>
-    </row>
-    <row r="552" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A552" s="1" t="s">
         <v>6</v>
       </c>
@@ -9938,7 +9933,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="553" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A553" s="1" t="s">
         <v>7</v>
       </c>
@@ -9955,7 +9950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="554" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A554" s="1" t="s">
         <v>8</v>
       </c>
@@ -9972,7 +9967,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="555" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A555" s="1" t="s">
         <v>9</v>
       </c>
@@ -9989,7 +9984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="556" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A556" s="1" t="s">
         <v>10</v>
       </c>
@@ -10006,7 +10001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="557" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A557" s="1" t="s">
         <v>11</v>
       </c>
@@ -10023,7 +10018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="558" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A558" s="1" t="s">
         <v>12</v>
       </c>
@@ -10040,7 +10035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="559" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A559" s="1" t="s">
         <v>13</v>
       </c>
@@ -10057,7 +10052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="560" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A560" s="1" t="s">
         <v>5</v>
       </c>
@@ -10618,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="593" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A593" s="1" t="s">
         <v>11</v>
       </c>
@@ -10635,7 +10630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="594" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A594" s="1" t="s">
         <v>12</v>
       </c>
@@ -10652,7 +10647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="595" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A595" s="1" t="s">
         <v>13</v>
       </c>
@@ -10669,7 +10664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="596" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
         <v>5</v>
       </c>
@@ -10685,9 +10680,8 @@
       <c r="E596" s="1">
         <v>1703</v>
       </c>
-      <c r="F596" s="1"/>
-    </row>
-    <row r="597" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="597" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A597" s="1" t="s">
         <v>6</v>
       </c>
@@ -10704,7 +10698,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="598" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A598" s="1" t="s">
         <v>7</v>
       </c>
@@ -10721,7 +10715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="599" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A599" s="1" t="s">
         <v>8</v>
       </c>
@@ -10738,7 +10732,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="600" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A600" s="1" t="s">
         <v>9</v>
       </c>
@@ -10755,7 +10749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="601" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A601" s="1" t="s">
         <v>10</v>
       </c>
@@ -10772,7 +10766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="602" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
         <v>11</v>
       </c>
@@ -10789,7 +10783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="603" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A603" s="1" t="s">
         <v>12</v>
       </c>
@@ -10806,7 +10800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="604" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A604" s="1" t="s">
         <v>13</v>
       </c>
@@ -10823,7 +10817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="605" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A605" s="1" t="s">
         <v>5</v>
       </c>
@@ -10840,7 +10834,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="606" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A606" s="1" t="s">
         <v>6</v>
       </c>
@@ -10857,7 +10851,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="607" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A607" s="1" t="s">
         <v>7</v>
       </c>
@@ -10874,7 +10868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="608" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A608" s="1" t="s">
         <v>8</v>
       </c>
@@ -11707,7 +11701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="657" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A657" s="1" t="s">
         <v>12</v>
       </c>
@@ -11724,7 +11718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="658" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A658" s="1" t="s">
         <v>13</v>
       </c>
@@ -11741,7 +11735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="659" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A659" s="1" t="s">
         <v>5</v>
       </c>
@@ -11758,7 +11752,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="660" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="660" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A660" s="1" t="s">
         <v>6</v>
       </c>
@@ -11775,7 +11769,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="661" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A661" s="1" t="s">
         <v>7</v>
       </c>
@@ -11792,7 +11786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="662" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A662" s="1" t="s">
         <v>8</v>
       </c>
@@ -11809,7 +11803,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="663" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A663" s="1" t="s">
         <v>9</v>
       </c>
@@ -11826,7 +11820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="664" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A664" s="1" t="s">
         <v>10</v>
       </c>
@@ -11843,7 +11837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="665" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A665" s="1" t="s">
         <v>11</v>
       </c>
@@ -11860,7 +11854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="666" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A666" s="1" t="s">
         <v>12</v>
       </c>
@@ -11877,7 +11871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="667" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="667" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A667" s="1" t="s">
         <v>13</v>
       </c>
@@ -11894,7 +11888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="668" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="668" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A668" s="1" t="s">
         <v>5</v>
       </c>
@@ -11910,9 +11904,8 @@
       <c r="E668" s="1">
         <v>594</v>
       </c>
-      <c r="F668" s="1"/>
-    </row>
-    <row r="669" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="669" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A669" s="1" t="s">
         <v>6</v>
       </c>
@@ -11929,7 +11922,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="670" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="670" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A670" s="1" t="s">
         <v>7</v>
       </c>
@@ -11946,7 +11939,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="671" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="671" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A671" s="1" t="s">
         <v>8</v>
       </c>
@@ -11963,7 +11956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="672" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="672" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A672" s="1" t="s">
         <v>9</v>
       </c>
@@ -12796,7 +12789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="721" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="721" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A721" s="1" t="s">
         <v>13</v>
       </c>
@@ -12813,7 +12806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="722" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="722" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A722" s="1" t="s">
         <v>5</v>
       </c>
@@ -12830,7 +12823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="723" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="723" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A723" s="1" t="s">
         <v>6</v>
       </c>
@@ -12847,7 +12840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="724" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="724" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A724" s="1" t="s">
         <v>7</v>
       </c>
@@ -12864,7 +12857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="725" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="725" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A725" s="1" t="s">
         <v>8</v>
       </c>
@@ -12881,7 +12874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="726" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="726" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A726" s="1" t="s">
         <v>9</v>
       </c>
@@ -12898,7 +12891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="727" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="727" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A727" s="1" t="s">
         <v>10</v>
       </c>
@@ -12915,7 +12908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="728" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="728" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A728" s="1" t="s">
         <v>11</v>
       </c>
@@ -12932,7 +12925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="729" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A729" s="1" t="s">
         <v>12</v>
       </c>
@@ -12949,7 +12942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="730" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="730" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A730" s="1" t="s">
         <v>13</v>
       </c>
@@ -12966,7 +12959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="731" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="731" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A731" s="1" t="s">
         <v>5</v>
       </c>
@@ -12982,9 +12975,8 @@
       <c r="E731" s="1">
         <v>9</v>
       </c>
-      <c r="F731" s="1"/>
-    </row>
-    <row r="732" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="732" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A732" s="1" t="s">
         <v>6</v>
       </c>
@@ -13001,7 +12993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="733" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="733" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A733" s="1" t="s">
         <v>7</v>
       </c>
@@ -13018,7 +13010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="734" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="734" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A734" s="1" t="s">
         <v>8</v>
       </c>
@@ -13035,7 +13027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="735" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="735" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A735" s="1" t="s">
         <v>9</v>
       </c>
@@ -13052,7 +13044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="736" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="736" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A736" s="1" t="s">
         <v>10</v>
       </c>
@@ -13613,7 +13605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="769" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="769" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A769" s="1" t="s">
         <v>7</v>
       </c>
@@ -13630,7 +13622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="770" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="770" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A770" s="1" t="s">
         <v>8</v>
       </c>
@@ -13647,7 +13639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="771" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A771" s="1" t="s">
         <v>9</v>
       </c>
@@ -13664,7 +13656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="772" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A772" s="1" t="s">
         <v>10</v>
       </c>
@@ -13681,7 +13673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="773" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A773" s="1" t="s">
         <v>11</v>
       </c>
@@ -13698,7 +13690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="774" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A774" s="1" t="s">
         <v>12</v>
       </c>
@@ -13715,7 +13707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="775" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A775" s="1" t="s">
         <v>13</v>
       </c>
@@ -13732,7 +13724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="776" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="776" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A776" s="1" t="s">
         <v>5</v>
       </c>
@@ -13748,9 +13740,8 @@
       <c r="E776" s="1">
         <v>1</v>
       </c>
-      <c r="F776" s="1"/>
-    </row>
-    <row r="777" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="777" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A777" s="1" t="s">
         <v>6</v>
       </c>
@@ -13767,7 +13758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="778" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="778" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A778" s="1" t="s">
         <v>7</v>
       </c>
@@ -13784,7 +13775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="779" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="779" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A779" s="1" t="s">
         <v>8</v>
       </c>
@@ -13801,7 +13792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="780" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="780" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A780" s="1" t="s">
         <v>9</v>
       </c>
@@ -13818,7 +13809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="781" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="781" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A781" s="1" t="s">
         <v>10</v>
       </c>
@@ -13835,7 +13826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="782" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="782" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A782" s="1" t="s">
         <v>11</v>
       </c>
@@ -13852,7 +13843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="783" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="783" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A783" s="1" t="s">
         <v>12</v>
       </c>
@@ -13869,7 +13860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="784" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="784" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A784" s="1" t="s">
         <v>13</v>
       </c>
@@ -14702,7 +14693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="833" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A833" s="1" t="s">
         <v>8</v>
       </c>
@@ -14719,7 +14710,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="834" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A834" s="1" t="s">
         <v>9</v>
       </c>
@@ -14736,7 +14727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="835" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A835" s="1" t="s">
         <v>10</v>
       </c>
@@ -14753,7 +14744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="836" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="836" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A836" s="1" t="s">
         <v>11</v>
       </c>
@@ -14770,7 +14761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="837" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A837" s="1" t="s">
         <v>12</v>
       </c>
@@ -14787,7 +14778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="838" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A838" s="1" t="s">
         <v>13</v>
       </c>
@@ -14804,7 +14795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="839" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="839" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A839" s="1" t="s">
         <v>5</v>
       </c>
@@ -14821,7 +14812,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="840" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A840" s="1" t="s">
         <v>6</v>
       </c>
@@ -14838,7 +14829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="841" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="841" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A841" s="1" t="s">
         <v>7</v>
       </c>
@@ -14855,7 +14846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="842" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="842" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A842" s="1" t="s">
         <v>8</v>
       </c>
@@ -14872,7 +14863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="843" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="843" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A843" s="1" t="s">
         <v>9</v>
       </c>
@@ -14889,7 +14880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="844" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="844" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A844" s="1" t="s">
         <v>10</v>
       </c>
@@ -14906,7 +14897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="845" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="845" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A845" s="1" t="s">
         <v>11</v>
       </c>
@@ -14923,7 +14914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="846" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="846" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A846" s="1" t="s">
         <v>12</v>
       </c>
@@ -14940,7 +14931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="847" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="847" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A847" s="1" t="s">
         <v>13</v>
       </c>
@@ -14957,7 +14948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="848" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="848" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A848" s="1" t="s">
         <v>5</v>
       </c>
@@ -14973,7 +14964,6 @@
       <c r="E848" s="1">
         <v>20</v>
       </c>
-      <c r="F848" s="1"/>
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A849" s="1" t="s">
@@ -16335,7 +16325,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="929" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="929" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A929" s="1" t="s">
         <v>5</v>
       </c>
@@ -16351,9 +16341,8 @@
       <c r="E929" s="1">
         <v>121</v>
       </c>
-      <c r="F929" s="1"/>
-    </row>
-    <row r="930" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="930" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A930" s="1" t="s">
         <v>6</v>
       </c>
@@ -16370,7 +16359,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="931" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="931" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A931" s="1" t="s">
         <v>7</v>
       </c>
@@ -16387,7 +16376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="932" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="932" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A932" s="1" t="s">
         <v>8</v>
       </c>
@@ -16404,7 +16393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="933" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="933" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A933" s="1" t="s">
         <v>9</v>
       </c>
@@ -16421,7 +16410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="934" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="934" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A934" s="1" t="s">
         <v>10</v>
       </c>
@@ -16438,7 +16427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="935" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="935" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A935" s="1" t="s">
         <v>11</v>
       </c>
@@ -16455,7 +16444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="936" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="936" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A936" s="1" t="s">
         <v>12</v>
       </c>
@@ -16472,7 +16461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="937" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="937" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A937" s="1" t="s">
         <v>13</v>
       </c>
@@ -16489,7 +16478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="938" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="938" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A938" s="1" t="s">
         <v>5</v>
       </c>
@@ -16506,7 +16495,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="939" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="939" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A939" s="1" t="s">
         <v>6</v>
       </c>
@@ -16523,7 +16512,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="940" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="940" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A940" s="1" t="s">
         <v>7</v>
       </c>
@@ -16540,7 +16529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="941" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="941" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A941" s="1" t="s">
         <v>8</v>
       </c>
@@ -16557,7 +16546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="942" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="942" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A942" s="1" t="s">
         <v>9</v>
       </c>
@@ -16574,7 +16563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="943" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="943" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A943" s="1" t="s">
         <v>10</v>
       </c>
@@ -16591,7 +16580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="944" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="944" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A944" s="1" t="s">
         <v>11</v>
       </c>
@@ -17968,7 +17957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1025" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1025" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1025" s="1" t="s">
         <v>11</v>
       </c>
@@ -17985,7 +17974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1026" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1026" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1026" s="1" t="s">
         <v>12</v>
       </c>
@@ -18002,7 +17991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1027" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1027" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1027" s="1" t="s">
         <v>13</v>
       </c>
@@ -18019,7 +18008,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1028" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1028" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1028" s="1" t="s">
         <v>5</v>
       </c>
@@ -18036,7 +18025,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="1029" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1029" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1029" s="1" t="s">
         <v>6</v>
       </c>
@@ -18053,7 +18042,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="1030" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1030" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1030" s="1" t="s">
         <v>7</v>
       </c>
@@ -18070,7 +18059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1031" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1031" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1031" s="1" t="s">
         <v>8</v>
       </c>
@@ -18087,7 +18076,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="1032" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1032" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1032" s="1" t="s">
         <v>9</v>
       </c>
@@ -18104,7 +18093,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="1033" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1033" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1033" s="1" t="s">
         <v>10</v>
       </c>
@@ -18121,7 +18110,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1034" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1034" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1034" s="1" t="s">
         <v>11</v>
       </c>
@@ -18138,7 +18127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1035" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1035" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1035" s="1" t="s">
         <v>12</v>
       </c>
@@ -18155,7 +18144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1036" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1036" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1036" s="1" t="s">
         <v>13</v>
       </c>
@@ -18172,7 +18161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1037" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1037" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1037" s="1" t="s">
         <v>5</v>
       </c>
@@ -18188,9 +18177,8 @@
       <c r="E1037" s="1">
         <v>366</v>
       </c>
-      <c r="F1037" s="1"/>
-    </row>
-    <row r="1038" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1038" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1038" s="1" t="s">
         <v>6</v>
       </c>
@@ -18207,7 +18195,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="1039" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1039" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1039" s="1" t="s">
         <v>7</v>
       </c>
@@ -18224,7 +18212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="1040" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1040" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1040" s="1" t="s">
         <v>8</v>
       </c>
@@ -19873,7 +19861,7 @@
         <v>2767</v>
       </c>
     </row>
-    <row r="1137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1137" s="1" t="s">
         <v>6</v>
       </c>
@@ -19890,7 +19878,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="1138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1138" s="1" t="s">
         <v>7</v>
       </c>
@@ -19907,7 +19895,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="1139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1139" s="1" t="s">
         <v>8</v>
       </c>
@@ -19924,7 +19912,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="1140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1140" s="1" t="s">
         <v>9</v>
       </c>
@@ -19941,7 +19929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="1141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1141" s="1" t="s">
         <v>10</v>
       </c>
@@ -19958,7 +19946,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1142" s="1" t="s">
         <v>11</v>
       </c>
@@ -19975,7 +19963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1143" s="1" t="s">
         <v>12</v>
       </c>
@@ -19992,7 +19980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1144" s="1" t="s">
         <v>13</v>
       </c>
@@ -20009,7 +19997,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="1145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1145" s="1" t="s">
         <v>5</v>
       </c>
@@ -20025,9 +20013,8 @@
       <c r="E1145" s="1">
         <v>3916</v>
       </c>
-      <c r="F1145" s="1"/>
-    </row>
-    <row r="1146" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1146" s="1" t="s">
         <v>6</v>
       </c>
@@ -20044,7 +20031,7 @@
         <v>3747</v>
       </c>
     </row>
-    <row r="1147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1147" s="1" t="s">
         <v>7</v>
       </c>
@@ -20061,7 +20048,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="1148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1148" s="1" t="s">
         <v>8</v>
       </c>
@@ -20078,7 +20065,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="1149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1149" s="1" t="s">
         <v>9</v>
       </c>
@@ -20095,7 +20082,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="1150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1150" s="1" t="s">
         <v>10</v>
       </c>
@@ -20112,7 +20099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1151" s="1" t="s">
         <v>11</v>
       </c>
@@ -20129,7 +20116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1152" s="1" t="s">
         <v>12</v>
       </c>
@@ -21778,7 +21765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1249" s="1" t="s">
         <v>10</v>
       </c>
@@ -21795,7 +21782,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1250" s="1" t="s">
         <v>11</v>
       </c>
@@ -21812,7 +21799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1251" s="1" t="s">
         <v>12</v>
       </c>
@@ -21829,7 +21816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1252" s="1" t="s">
         <v>13</v>
       </c>
@@ -21846,7 +21833,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="1253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1253" s="1" t="s">
         <v>5</v>
       </c>
@@ -21862,9 +21849,8 @@
       <c r="E1253" s="1">
         <v>9</v>
       </c>
-      <c r="F1253" s="1"/>
-    </row>
-    <row r="1254" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1254" s="1" t="s">
         <v>6</v>
       </c>
@@ -21881,7 +21867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1255" s="1" t="s">
         <v>7</v>
       </c>
@@ -21898,7 +21884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1256" s="1" t="s">
         <v>8</v>
       </c>
@@ -21915,7 +21901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1257" s="1" t="s">
         <v>9</v>
       </c>
@@ -21932,7 +21918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1258" s="1" t="s">
         <v>10</v>
       </c>
@@ -21949,7 +21935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1259" s="1" t="s">
         <v>11</v>
       </c>
@@ -21966,7 +21952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1260" s="1" t="s">
         <v>12</v>
       </c>
@@ -21983,7 +21969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1261" s="1" t="s">
         <v>13</v>
       </c>
@@ -22000,7 +21986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1262" s="1" t="s">
         <v>5</v>
       </c>
@@ -22017,7 +22003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1263" s="1" t="s">
         <v>6</v>
       </c>
@@ -22034,7 +22020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1264" s="1" t="s">
         <v>7</v>
       </c>
@@ -23683,7 +23669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1361" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1361" s="1" t="s">
         <v>5</v>
       </c>
@@ -23699,9 +23685,8 @@
       <c r="E1361" s="1">
         <v>244</v>
       </c>
-      <c r="F1361" s="1"/>
-    </row>
-    <row r="1362" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1362" s="1" t="s">
         <v>6</v>
       </c>
@@ -23718,7 +23703,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="1363" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1363" s="1" t="s">
         <v>7</v>
       </c>
@@ -23735,7 +23720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1364" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1364" s="1" t="s">
         <v>8</v>
       </c>
@@ -23752,7 +23737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1365" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1365" s="1" t="s">
         <v>9</v>
       </c>
@@ -23769,7 +23754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1366" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1366" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1366" s="1" t="s">
         <v>10</v>
       </c>
@@ -23786,7 +23771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1367" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1367" s="1" t="s">
         <v>11</v>
       </c>
@@ -23803,7 +23788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1368" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1368" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1368" s="1" t="s">
         <v>12</v>
       </c>
@@ -23820,7 +23805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1369" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1369" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1369" s="1" t="s">
         <v>13</v>
       </c>
@@ -23837,7 +23822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1370" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1370" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1370" s="1" t="s">
         <v>5</v>
       </c>
@@ -23854,7 +23839,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="1371" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1371" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1371" s="1" t="s">
         <v>6</v>
       </c>
@@ -23871,7 +23856,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="1372" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1372" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1372" s="1" t="s">
         <v>7</v>
       </c>
@@ -23888,7 +23873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1373" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1373" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1373" s="1" t="s">
         <v>8</v>
       </c>
@@ -23905,7 +23890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1374" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1374" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1374" s="1" t="s">
         <v>9</v>
       </c>
@@ -23922,7 +23907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1375" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1375" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1375" s="1" t="s">
         <v>10</v>
       </c>
@@ -23939,7 +23924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1376" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1376" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1376" s="1" t="s">
         <v>11</v>
       </c>
@@ -25316,7 +25301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1457" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1457" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1457" s="1" t="s">
         <v>11</v>
       </c>
@@ -25333,7 +25318,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="1458" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1458" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1458" s="1" t="s">
         <v>12</v>
       </c>
@@ -25350,7 +25335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1459" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1459" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1459" s="1" t="s">
         <v>13</v>
       </c>
@@ -25367,7 +25352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1460" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1460" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1460" s="1" t="s">
         <v>5</v>
       </c>
@@ -25384,7 +25369,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="1461" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1461" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1461" s="1" t="s">
         <v>6</v>
       </c>
@@ -25401,7 +25386,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="1462" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1462" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1462" s="1" t="s">
         <v>7</v>
       </c>
@@ -25418,7 +25403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1463" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1463" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1463" s="1" t="s">
         <v>8</v>
       </c>
@@ -25435,7 +25420,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="1464" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1464" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1464" s="1" t="s">
         <v>9</v>
       </c>
@@ -25452,7 +25437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1465" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1465" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1465" s="1" t="s">
         <v>10</v>
       </c>
@@ -25469,7 +25454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1466" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1466" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1466" s="1" t="s">
         <v>11</v>
       </c>
@@ -25486,7 +25471,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="1467" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1467" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1467" s="1" t="s">
         <v>12</v>
       </c>
@@ -25503,7 +25488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1468" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1468" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1468" s="1" t="s">
         <v>13</v>
       </c>
@@ -25520,7 +25505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1469" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1469" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1469" s="1" t="s">
         <v>5</v>
       </c>
@@ -25536,9 +25521,8 @@
       <c r="E1469" s="1">
         <v>433</v>
       </c>
-      <c r="F1469" s="1"/>
-    </row>
-    <row r="1470" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1470" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1470" s="1" t="s">
         <v>6</v>
       </c>
@@ -25555,7 +25539,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="1471" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1471" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1471" s="1" t="s">
         <v>7</v>
       </c>
@@ -25572,7 +25556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1472" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1472" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1472" s="1" t="s">
         <v>8</v>
       </c>
@@ -27221,7 +27205,7 @@
         <v>4256</v>
       </c>
     </row>
-    <row r="1569" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1569" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1569" s="1" t="s">
         <v>6</v>
       </c>
@@ -27238,7 +27222,7 @@
         <v>2851</v>
       </c>
     </row>
-    <row r="1570" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1570" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1570" s="1" t="s">
         <v>7</v>
       </c>
@@ -27255,7 +27239,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1571" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1571" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1571" s="1" t="s">
         <v>8</v>
       </c>
@@ -27272,7 +27256,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="1572" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1572" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1572" s="1" t="s">
         <v>9</v>
       </c>
@@ -27289,7 +27273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1573" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1573" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1573" s="1" t="s">
         <v>10</v>
       </c>
@@ -27306,7 +27290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1574" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1574" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1574" s="1" t="s">
         <v>11</v>
       </c>
@@ -27323,7 +27307,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="1575" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1575" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1575" s="1" t="s">
         <v>12</v>
       </c>
@@ -27340,7 +27324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1576" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1576" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1576" s="1" t="s">
         <v>13</v>
       </c>
@@ -27357,7 +27341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="1577" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1577" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1577" s="1" t="s">
         <v>5</v>
       </c>
@@ -27373,9 +27357,8 @@
       <c r="E1577" s="1">
         <v>24385</v>
       </c>
-      <c r="F1577" s="1"/>
-    </row>
-    <row r="1578" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1578" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1578" s="1" t="s">
         <v>6</v>
       </c>
@@ -27392,7 +27375,7 @@
         <v>19428</v>
       </c>
     </row>
-    <row r="1579" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1579" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1579" s="1" t="s">
         <v>7</v>
       </c>
@@ -27409,7 +27392,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="1580" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1580" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1580" s="1" t="s">
         <v>8</v>
       </c>
@@ -27426,7 +27409,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="1581" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1581" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1581" s="1" t="s">
         <v>9</v>
       </c>
@@ -27443,7 +27426,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="1582" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1582" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1582" s="1" t="s">
         <v>10</v>
       </c>
@@ -27460,7 +27443,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1583" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1583" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1583" s="1" t="s">
         <v>11</v>
       </c>
@@ -27477,7 +27460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1584" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1584" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1584" s="1" t="s">
         <v>12</v>
       </c>
@@ -29126,7 +29109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1681" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1681" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1681" s="1" t="s">
         <v>10</v>
       </c>
@@ -29143,7 +29126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1682" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1682" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1682" s="1" t="s">
         <v>11</v>
       </c>
@@ -29160,7 +29143,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="1683" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1683" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1683" s="1" t="s">
         <v>12</v>
       </c>
@@ -29177,7 +29160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1684" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1684" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1684" s="1" t="s">
         <v>13</v>
       </c>
@@ -29194,7 +29177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1685" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1685" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1685" s="1" t="s">
         <v>5</v>
       </c>
@@ -29210,9 +29193,8 @@
       <c r="E1685" s="1">
         <v>91642</v>
       </c>
-      <c r="F1685" s="1"/>
-    </row>
-    <row r="1686" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1686" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1686" s="1" t="s">
         <v>6</v>
       </c>
@@ -29229,7 +29211,7 @@
         <v>78803</v>
       </c>
     </row>
-    <row r="1687" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1687" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1687" s="1" t="s">
         <v>7</v>
       </c>
@@ -29246,7 +29228,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="1688" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1688" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1688" s="1" t="s">
         <v>8</v>
       </c>
@@ -29263,7 +29245,7 @@
         <v>3831</v>
       </c>
     </row>
-    <row r="1689" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1689" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1689" s="1" t="s">
         <v>9</v>
       </c>
@@ -29280,7 +29262,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="1690" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1690" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1690" s="1" t="s">
         <v>10</v>
       </c>
@@ -29297,7 +29279,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="1691" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1691" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1691" s="1" t="s">
         <v>11</v>
       </c>
@@ -29314,7 +29296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1692" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1692" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1692" s="1" t="s">
         <v>12</v>
       </c>
@@ -29331,7 +29313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1693" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1693" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1693" s="1" t="s">
         <v>13</v>
       </c>
@@ -29348,7 +29330,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="1694" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1694" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1694" s="1" t="s">
         <v>5</v>
       </c>
@@ -29365,7 +29347,7 @@
         <v>95721</v>
       </c>
     </row>
-    <row r="1695" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1695" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1695" s="1" t="s">
         <v>6</v>
       </c>
@@ -29382,7 +29364,7 @@
         <v>79409</v>
       </c>
     </row>
-    <row r="1696" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1696" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1696" s="1" t="s">
         <v>7</v>
       </c>
@@ -32935,7 +32917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1905" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1905" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1905" s="1" t="s">
         <v>9</v>
       </c>
@@ -32952,7 +32934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1906" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1906" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1906" s="1" t="s">
         <v>10</v>
       </c>
@@ -32969,7 +32951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1907" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1907" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1907" s="1" t="s">
         <v>11</v>
       </c>
@@ -32986,7 +32968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1908" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1908" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1908" s="1" t="s">
         <v>12</v>
       </c>
@@ -33003,7 +32985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1909" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1909" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1909" s="1" t="s">
         <v>13</v>
       </c>
@@ -33020,7 +33002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1910" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1910" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1910" s="1" t="s">
         <v>5</v>
       </c>
@@ -33036,9 +33018,8 @@
       <c r="E1910" s="1">
         <v>0</v>
       </c>
-      <c r="F1910" s="1"/>
-    </row>
-    <row r="1911" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1911" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1911" s="1" t="s">
         <v>6</v>
       </c>
@@ -33055,7 +33036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1912" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1912" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1912" s="1" t="s">
         <v>7</v>
       </c>
@@ -33072,7 +33053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1913" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1913" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1913" s="1" t="s">
         <v>8</v>
       </c>
@@ -33089,7 +33070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1914" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1914" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1914" s="1" t="s">
         <v>9</v>
       </c>
@@ -33106,7 +33087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1915" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1915" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1915" s="1" t="s">
         <v>10</v>
       </c>
@@ -33123,7 +33104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1916" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1916" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1916" s="1" t="s">
         <v>11</v>
       </c>
@@ -33140,7 +33121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1917" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1917" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1917" s="1" t="s">
         <v>12</v>
       </c>
@@ -33157,7 +33138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1918" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1918" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1918" s="1" t="s">
         <v>13</v>
       </c>
@@ -33174,7 +33155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1919" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1919" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1919" s="1" t="s">
         <v>5</v>
       </c>
@@ -33191,7 +33172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1920" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1920" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1920" s="1" t="s">
         <v>6</v>
       </c>
@@ -33752,7 +33733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1953" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1953" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1953" s="1" t="s">
         <v>12</v>
       </c>
@@ -33769,7 +33750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1954" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1954" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1954" s="1" t="s">
         <v>13</v>
       </c>
@@ -33786,7 +33767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1955" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1955" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1955" s="1" t="s">
         <v>5</v>
       </c>
@@ -33802,9 +33783,8 @@
       <c r="E1955" s="1">
         <v>0</v>
       </c>
-      <c r="F1955" s="1"/>
-    </row>
-    <row r="1956" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1956" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1956" s="1" t="s">
         <v>6</v>
       </c>
@@ -33821,7 +33801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1957" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1957" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1957" s="1" t="s">
         <v>7</v>
       </c>
@@ -33838,7 +33818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1958" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1958" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1958" s="1" t="s">
         <v>8</v>
       </c>
@@ -33855,7 +33835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1959" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1959" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1959" s="1" t="s">
         <v>9</v>
       </c>
@@ -33872,7 +33852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1960" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1960" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1960" s="1" t="s">
         <v>10</v>
       </c>
@@ -33889,7 +33869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1961" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1961" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1961" s="1" t="s">
         <v>11</v>
       </c>
@@ -33906,7 +33886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1962" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1962" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1962" s="1" t="s">
         <v>12</v>
       </c>
@@ -33923,7 +33903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1963" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1963" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1963" s="1" t="s">
         <v>13</v>
       </c>
@@ -33940,7 +33920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1964" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1964" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1964" s="1" t="s">
         <v>5</v>
       </c>
@@ -33957,7 +33937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1965" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1965" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1965" s="1" t="s">
         <v>6</v>
       </c>
@@ -33974,7 +33954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1966" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1966" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1966" s="1" t="s">
         <v>7</v>
       </c>
@@ -33991,7 +33971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1967" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1967" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1967" s="1" t="s">
         <v>8</v>
       </c>
@@ -34008,7 +33988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1968" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1968" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1968" s="1" t="s">
         <v>9</v>
       </c>
@@ -34841,7 +34821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2017" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2017" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2017" s="1" t="s">
         <v>13</v>
       </c>
@@ -34858,7 +34838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2018" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2018" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2018" s="1" t="s">
         <v>5</v>
       </c>
@@ -34875,7 +34855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2019" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2019" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2019" s="1" t="s">
         <v>6</v>
       </c>
@@ -34892,7 +34872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2020" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2020" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2020" s="1" t="s">
         <v>7</v>
       </c>
@@ -34909,7 +34889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2021" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2021" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2021" s="1" t="s">
         <v>8</v>
       </c>
@@ -34926,7 +34906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2022" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2022" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2022" s="1" t="s">
         <v>9</v>
       </c>
@@ -34943,7 +34923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2023" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2023" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2023" s="1" t="s">
         <v>10</v>
       </c>
@@ -34960,7 +34940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2024" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2024" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2024" s="1" t="s">
         <v>11</v>
       </c>
@@ -34977,7 +34957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2025" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2025" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2025" s="1" t="s">
         <v>12</v>
       </c>
@@ -34994,7 +34974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2026" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2026" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2026" s="1" t="s">
         <v>13</v>
       </c>
@@ -35011,7 +34991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2027" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2027" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2027" s="1" t="s">
         <v>5</v>
       </c>
@@ -35027,9 +35007,8 @@
       <c r="E2027" s="1">
         <v>0</v>
       </c>
-      <c r="F2027" s="1"/>
-    </row>
-    <row r="2028" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2028" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2028" s="1" t="s">
         <v>6</v>
       </c>
@@ -35046,7 +35025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2029" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2029" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2029" s="1" t="s">
         <v>7</v>
       </c>
@@ -35063,7 +35042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2030" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2030" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2030" s="1" t="s">
         <v>8</v>
       </c>
@@ -35080,7 +35059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2031" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2031" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2031" s="1" t="s">
         <v>9</v>
       </c>
@@ -35097,7 +35076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2032" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2032" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2032" s="1" t="s">
         <v>10</v>
       </c>
@@ -41098,7 +41077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2385" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2385" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2385" s="1" t="s">
         <v>12</v>
       </c>
@@ -41115,7 +41094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2386" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2386" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2386" s="1" t="s">
         <v>13</v>
       </c>
@@ -41132,7 +41111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2387" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2387" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2387" s="1" t="s">
         <v>5</v>
       </c>
@@ -41149,7 +41128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2388" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2388" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2388" s="1" t="s">
         <v>6</v>
       </c>
@@ -41166,7 +41145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2389" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2389" s="1" t="s">
         <v>7</v>
       </c>
@@ -41183,7 +41162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2390" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2390" s="1" t="s">
         <v>8</v>
       </c>
@@ -41200,7 +41179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2391" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2391" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2391" s="1" t="s">
         <v>9</v>
       </c>
@@ -41217,7 +41196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2392" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2392" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2392" s="1" t="s">
         <v>10</v>
       </c>
@@ -41234,7 +41213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2393" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2393" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2393" s="1" t="s">
         <v>11</v>
       </c>
@@ -41251,7 +41230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2394" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2394" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2394" s="1" t="s">
         <v>12</v>
       </c>
@@ -41268,7 +41247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2395" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2395" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2395" s="1" t="s">
         <v>13</v>
       </c>
@@ -41285,7 +41264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2396" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2396" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2396" s="1" t="s">
         <v>5</v>
       </c>
@@ -41301,9 +41280,8 @@
       <c r="E2396" s="1">
         <v>2</v>
       </c>
-      <c r="F2396" s="1"/>
-    </row>
-    <row r="2397" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2397" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2397" s="1" t="s">
         <v>6</v>
       </c>
@@ -41320,7 +41298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2398" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2398" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2398" s="1" t="s">
         <v>7</v>
       </c>
@@ -41337,7 +41315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2399" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2399" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2399" s="1" t="s">
         <v>8</v>
       </c>
@@ -41354,7 +41332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2400" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2400" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2400" s="1" t="s">
         <v>9</v>
       </c>
@@ -43003,7 +42981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2497" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2497" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2497" s="1" t="s">
         <v>7</v>
       </c>
@@ -43020,7 +42998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2498" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2498" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2498" s="1" t="s">
         <v>8</v>
       </c>
@@ -43037,7 +43015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2499" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2499" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2499" s="1" t="s">
         <v>9</v>
       </c>
@@ -43054,7 +43032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2500" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2500" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2500" s="1" t="s">
         <v>10</v>
       </c>
@@ -43071,7 +43049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2501" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2501" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2501" s="1" t="s">
         <v>11</v>
       </c>
@@ -43088,7 +43066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2502" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2502" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2502" s="1" t="s">
         <v>12</v>
       </c>
@@ -43105,7 +43083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2503" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2503" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2503" s="1" t="s">
         <v>13</v>
       </c>
@@ -43122,7 +43100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2504" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2504" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2504" s="1" t="s">
         <v>5</v>
       </c>
@@ -43138,9 +43116,8 @@
       <c r="E2504" s="1">
         <v>1</v>
       </c>
-      <c r="F2504" s="1"/>
-    </row>
-    <row r="2505" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2505" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2505" s="1" t="s">
         <v>6</v>
       </c>
@@ -43157,7 +43134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2506" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2506" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2506" s="1" t="s">
         <v>7</v>
       </c>
@@ -43174,7 +43151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2507" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2507" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2507" s="1" t="s">
         <v>8</v>
       </c>
@@ -43191,7 +43168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2508" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2508" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2508" s="1" t="s">
         <v>9</v>
       </c>
@@ -43208,7 +43185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2509" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2509" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2509" s="1" t="s">
         <v>10</v>
       </c>
@@ -43225,7 +43202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2510" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2510" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2510" s="1" t="s">
         <v>11</v>
       </c>
@@ -43242,7 +43219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2511" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2511" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2511" s="1" t="s">
         <v>12</v>
       </c>
@@ -43259,7 +43236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2512" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2512" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2512" s="1" t="s">
         <v>13</v>
       </c>
@@ -44908,7 +44885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2609" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2609" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2609" s="1" t="s">
         <v>11</v>
       </c>
@@ -44925,7 +44902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2610" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2610" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2610" s="1" t="s">
         <v>12</v>
       </c>
@@ -44942,7 +44919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2611" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2611" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2611" s="1" t="s">
         <v>13</v>
       </c>
@@ -44959,7 +44936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2612" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2612" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2612" s="1" t="s">
         <v>5</v>
       </c>
@@ -44975,9 +44952,8 @@
       <c r="E2612" s="1">
         <v>0</v>
       </c>
-      <c r="F2612" s="1"/>
-    </row>
-    <row r="2613" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2613" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2613" s="1" t="s">
         <v>6</v>
       </c>
@@ -44994,7 +44970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2614" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2614" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2614" s="1" t="s">
         <v>7</v>
       </c>
@@ -45011,7 +44987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2615" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2615" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2615" s="1" t="s">
         <v>8</v>
       </c>
@@ -45028,7 +45004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2616" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2616" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2616" s="1" t="s">
         <v>9</v>
       </c>
@@ -45045,7 +45021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2617" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2617" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2617" s="1" t="s">
         <v>10</v>
       </c>
@@ -45062,7 +45038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2618" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2618" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2618" s="1" t="s">
         <v>11</v>
       </c>
@@ -45079,7 +45055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2619" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2619" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2619" s="1" t="s">
         <v>12</v>
       </c>
@@ -45096,7 +45072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2620" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2620" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2620" s="1" t="s">
         <v>13</v>
       </c>
@@ -45113,7 +45089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2621" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2621" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2621" s="1" t="s">
         <v>5</v>
       </c>
@@ -45130,7 +45106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2622" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2622" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2622" s="1" t="s">
         <v>6</v>
       </c>
@@ -45147,7 +45123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2623" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2623" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2623" s="1" t="s">
         <v>7</v>
       </c>
@@ -45164,7 +45140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2624" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2624" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2624" s="1" t="s">
         <v>8</v>
       </c>
@@ -46541,7 +46517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2705" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2705" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2705" s="1" t="s">
         <v>8</v>
       </c>
@@ -46558,7 +46534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2706" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2706" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2706" s="1" t="s">
         <v>9</v>
       </c>
@@ -46575,7 +46551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2707" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2707" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2707" s="1" t="s">
         <v>10</v>
       </c>
@@ -46592,7 +46568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2708" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2708" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2708" s="1" t="s">
         <v>11</v>
       </c>
@@ -46609,7 +46585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2709" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2709" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2709" s="1" t="s">
         <v>12</v>
       </c>
@@ -46626,7 +46602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2710" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2710" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2710" s="1" t="s">
         <v>13</v>
       </c>
@@ -46643,7 +46619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2711" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2711" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2711" s="1" t="s">
         <v>5</v>
       </c>
@@ -46660,7 +46636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2712" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2712" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2712" s="1" t="s">
         <v>6</v>
       </c>
@@ -46677,7 +46653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2713" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2713" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2713" s="1" t="s">
         <v>7</v>
       </c>
@@ -46694,7 +46670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2714" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2714" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2714" s="1" t="s">
         <v>8</v>
       </c>
@@ -46711,7 +46687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2715" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2715" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2715" s="1" t="s">
         <v>9</v>
       </c>
@@ -46728,7 +46704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2716" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2716" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2716" s="1" t="s">
         <v>10</v>
       </c>
@@ -46745,7 +46721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2717" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2717" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2717" s="1" t="s">
         <v>11</v>
       </c>
@@ -46762,7 +46738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2718" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2718" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2718" s="1" t="s">
         <v>12</v>
       </c>
@@ -46779,7 +46755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2719" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2719" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2719" s="1" t="s">
         <v>13</v>
       </c>
@@ -46796,7 +46772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2720" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2720" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2720" s="1" t="s">
         <v>5</v>
       </c>
@@ -46812,7 +46788,6 @@
       <c r="E2720" s="1">
         <v>0</v>
       </c>
-      <c r="F2720" s="1"/>
     </row>
     <row r="2721" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2721" s="1" t="s">
@@ -48446,7 +48421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2817" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2817" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2817" s="1" t="s">
         <v>12</v>
       </c>
@@ -48463,7 +48438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2818" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2818" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2818" s="1" t="s">
         <v>13</v>
       </c>
@@ -48480,7 +48455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2819" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2819" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2819" s="1" t="s">
         <v>5</v>
       </c>
@@ -48497,7 +48472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2820" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2820" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2820" s="1" t="s">
         <v>6</v>
       </c>
@@ -48514,7 +48489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2821" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2821" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2821" s="1" t="s">
         <v>7</v>
       </c>
@@ -48531,7 +48506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2822" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2822" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2822" s="1" t="s">
         <v>8</v>
       </c>
@@ -48548,7 +48523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2823" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2823" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2823" s="1" t="s">
         <v>9</v>
       </c>
@@ -48565,7 +48540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2824" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2824" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2824" s="1" t="s">
         <v>10</v>
       </c>
@@ -48582,7 +48557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2825" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2825" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2825" s="1" t="s">
         <v>11</v>
       </c>
@@ -48599,7 +48574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2826" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2826" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2826" s="1" t="s">
         <v>12</v>
       </c>
@@ -48616,7 +48591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2827" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2827" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2827" s="1" t="s">
         <v>13</v>
       </c>
@@ -48633,7 +48608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2828" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2828" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2828" s="1" t="s">
         <v>5</v>
       </c>
@@ -48649,9 +48624,8 @@
       <c r="E2828" s="1">
         <v>17</v>
       </c>
-      <c r="F2828" s="1"/>
-    </row>
-    <row r="2829" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2829" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2829" s="1" t="s">
         <v>6</v>
       </c>
@@ -48668,7 +48642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2830" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2830" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2830" s="1" t="s">
         <v>7</v>
       </c>
@@ -48685,7 +48659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2831" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2831" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2831" s="1" t="s">
         <v>8</v>
       </c>
@@ -48702,7 +48676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2832" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2832" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2832" s="1" t="s">
         <v>9</v>
       </c>
@@ -50351,7 +50325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2929" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2929" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2929" s="1" t="s">
         <v>7</v>
       </c>
@@ -50368,7 +50342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2930" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2930" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2930" s="1" t="s">
         <v>8</v>
       </c>
@@ -50385,7 +50359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2931" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2931" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2931" s="1" t="s">
         <v>9</v>
       </c>
@@ -50402,7 +50376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2932" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2932" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2932" s="1" t="s">
         <v>10</v>
       </c>
@@ -50419,7 +50393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2933" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2933" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2933" s="1" t="s">
         <v>11</v>
       </c>
@@ -50436,7 +50410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2934" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2934" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2934" s="1" t="s">
         <v>12</v>
       </c>
@@ -50453,7 +50427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2935" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2935" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2935" s="1" t="s">
         <v>13</v>
       </c>
@@ -50470,7 +50444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2936" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2936" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2936" s="1" t="s">
         <v>5</v>
       </c>
@@ -50486,9 +50460,8 @@
       <c r="E2936" s="1">
         <v>0</v>
       </c>
-      <c r="F2936" s="1"/>
-    </row>
-    <row r="2937" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2937" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2937" s="1" t="s">
         <v>6</v>
       </c>
@@ -50505,7 +50478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2938" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2938" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2938" s="1" t="s">
         <v>7</v>
       </c>
@@ -50522,7 +50495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2939" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2939" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2939" s="1" t="s">
         <v>8</v>
       </c>
@@ -50539,7 +50512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2940" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2940" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2940" s="1" t="s">
         <v>9</v>
       </c>
@@ -50556,7 +50529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2941" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2941" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2941" s="1" t="s">
         <v>10</v>
       </c>
@@ -50573,7 +50546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2942" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2942" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2942" s="1" t="s">
         <v>11</v>
       </c>
@@ -50590,7 +50563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2943" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2943" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2943" s="1" t="s">
         <v>12</v>
       </c>
@@ -50607,7 +50580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2944" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2944" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2944" s="1" t="s">
         <v>13</v>
       </c>
@@ -52256,7 +52229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3041" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3041" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3041" s="1" t="s">
         <v>11</v>
       </c>
@@ -52273,7 +52246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3042" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3042" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3042" s="1" t="s">
         <v>12</v>
       </c>
@@ -52290,7 +52263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3043" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3043" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3043" s="1" t="s">
         <v>13</v>
       </c>
@@ -52307,7 +52280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3044" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3044" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3044" s="1" t="s">
         <v>5</v>
       </c>
@@ -52323,9 +52296,8 @@
       <c r="E3044" s="1">
         <v>52</v>
       </c>
-      <c r="F3044" s="1"/>
-    </row>
-    <row r="3045" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3045" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3045" s="1" t="s">
         <v>6</v>
       </c>
@@ -52342,7 +52314,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3046" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3046" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3046" s="1" t="s">
         <v>7</v>
       </c>
@@ -52359,7 +52331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3047" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3047" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3047" s="1" t="s">
         <v>8</v>
       </c>
@@ -52376,7 +52348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3048" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3048" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3048" s="1" t="s">
         <v>9</v>
       </c>
@@ -52393,7 +52365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3049" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3049" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3049" s="1" t="s">
         <v>10</v>
       </c>
@@ -52410,7 +52382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3050" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3050" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3050" s="1" t="s">
         <v>11</v>
       </c>
@@ -52427,7 +52399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3051" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3051" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3051" s="1" t="s">
         <v>12</v>
       </c>
@@ -52444,7 +52416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3052" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3052" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3052" s="1" t="s">
         <v>13</v>
       </c>
@@ -52461,7 +52433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3053" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3053" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3053" s="1" t="s">
         <v>5</v>
       </c>
@@ -52478,7 +52450,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3054" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3054" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3054" s="1" t="s">
         <v>6</v>
       </c>
@@ -52495,7 +52467,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3055" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3055" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3055" s="1" t="s">
         <v>7</v>
       </c>
@@ -52512,7 +52484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3056" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3056" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3056" s="1" t="s">
         <v>8</v>
       </c>
@@ -53889,7 +53861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3137" s="1" t="s">
         <v>8</v>
       </c>
@@ -53906,7 +53878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3138" s="1" t="s">
         <v>9</v>
       </c>
@@ -53923,7 +53895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3139" s="1" t="s">
         <v>10</v>
       </c>
@@ -53940,7 +53912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3140" s="1" t="s">
         <v>11</v>
       </c>
@@ -53957,7 +53929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3141" s="1" t="s">
         <v>12</v>
       </c>
@@ -53974,7 +53946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3142" s="1" t="s">
         <v>13</v>
       </c>
@@ -53991,7 +53963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3143" s="1" t="s">
         <v>5</v>
       </c>
@@ -54008,7 +53980,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3144" s="1" t="s">
         <v>6</v>
       </c>
@@ -54025,7 +53997,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3145" s="1" t="s">
         <v>7</v>
       </c>
@@ -54042,7 +54014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3146" s="1" t="s">
         <v>8</v>
       </c>
@@ -54059,7 +54031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3147" s="1" t="s">
         <v>9</v>
       </c>
@@ -54076,7 +54048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3148" s="1" t="s">
         <v>10</v>
       </c>
@@ -54093,7 +54065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3149" s="1" t="s">
         <v>11</v>
       </c>
@@ -54110,7 +54082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3150" s="1" t="s">
         <v>12</v>
       </c>
@@ -54127,7 +54099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3151" s="1" t="s">
         <v>13</v>
       </c>
@@ -54144,7 +54116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3152" s="1" t="s">
         <v>5</v>
       </c>
@@ -54160,7 +54132,6 @@
       <c r="E3152" s="1">
         <v>58</v>
       </c>
-      <c r="F3152" s="1"/>
     </row>
     <row r="3153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3153" s="1" t="s">
@@ -56066,7 +56037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3265" s="1" t="s">
         <v>10</v>
       </c>
@@ -56083,7 +56054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3266" s="1" t="s">
         <v>11</v>
       </c>
@@ -56100,7 +56071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3267" s="1" t="s">
         <v>12</v>
       </c>
@@ -56117,7 +56088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3268" s="1" t="s">
         <v>13</v>
       </c>
@@ -56134,7 +56105,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3269" s="1" t="s">
         <v>5</v>
       </c>
@@ -56150,9 +56121,8 @@
       <c r="E3269">
         <v>893</v>
       </c>
-      <c r="F3269" s="1"/>
-    </row>
-    <row r="3270" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3270" s="1" t="s">
         <v>6</v>
       </c>
@@ -56169,7 +56139,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="3271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3271" s="1" t="s">
         <v>7</v>
       </c>
@@ -56186,7 +56156,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3272" s="1" t="s">
         <v>8</v>
       </c>
@@ -56203,7 +56173,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3273" s="1" t="s">
         <v>9</v>
       </c>
@@ -56220,7 +56190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3274" s="1" t="s">
         <v>10</v>
       </c>
@@ -56237,7 +56207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3275" s="1" t="s">
         <v>11</v>
       </c>
@@ -56254,7 +56224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3276" s="1" t="s">
         <v>12</v>
       </c>
@@ -56271,7 +56241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3277" s="1" t="s">
         <v>13</v>
       </c>
@@ -56288,7 +56258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3278" s="1" t="s">
         <v>5</v>
       </c>
@@ -56305,7 +56275,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="3279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3279" s="1" t="s">
         <v>6</v>
       </c>
@@ -56322,7 +56292,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="3280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3280" s="1" t="s">
         <v>7</v>
       </c>
@@ -57155,7 +57125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3329" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3329" s="1" t="s">
         <v>11</v>
       </c>
@@ -57172,7 +57142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3330" s="1" t="s">
         <v>12</v>
       </c>
@@ -57189,7 +57159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3331" s="1" t="s">
         <v>13</v>
       </c>
@@ -57206,7 +57176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3332" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3332" s="1" t="s">
         <v>5</v>
       </c>
@@ -57223,7 +57193,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="3333" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3333" s="1" t="s">
         <v>6</v>
       </c>
@@ -57240,7 +57210,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3334" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3334" s="1" t="s">
         <v>7</v>
       </c>
@@ -57257,7 +57227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3335" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3335" s="1" t="s">
         <v>8</v>
       </c>
@@ -57274,7 +57244,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3336" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3336" s="1" t="s">
         <v>9</v>
       </c>
@@ -57291,7 +57261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3337" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3337" s="1" t="s">
         <v>10</v>
       </c>
@@ -57308,7 +57278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3338" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3338" s="1" t="s">
         <v>11</v>
       </c>
@@ -57325,7 +57295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3339" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3339" s="1" t="s">
         <v>12</v>
       </c>
@@ -57342,7 +57312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3340" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3340" s="1" t="s">
         <v>13</v>
       </c>
@@ -57359,7 +57329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3341" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3341" s="1" t="s">
         <v>5</v>
       </c>
@@ -57375,9 +57345,8 @@
       <c r="E3341">
         <v>1147</v>
       </c>
-      <c r="F3341" s="1"/>
-    </row>
-    <row r="3342" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3342" s="1" t="s">
         <v>6</v>
       </c>
@@ -57394,7 +57363,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="3343" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3343" s="1" t="s">
         <v>7</v>
       </c>
@@ -57411,7 +57380,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3344" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3344" s="1" t="s">
         <v>8</v>
       </c>
@@ -58516,7 +58485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3409" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3409" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3409" s="1" t="s">
         <v>10</v>
       </c>
@@ -58533,7 +58502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3410" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3410" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3410" s="1" t="s">
         <v>11</v>
       </c>
@@ -58550,7 +58519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3411" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3411" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3411" s="1" t="s">
         <v>12</v>
       </c>
@@ -58567,7 +58536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3412" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3412" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3412" s="1" t="s">
         <v>13</v>
       </c>
@@ -58584,7 +58553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3413" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3413" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3413" s="1" t="s">
         <v>5</v>
       </c>
@@ -58600,9 +58569,8 @@
       <c r="E3413">
         <v>687</v>
       </c>
-      <c r="F3413" s="1"/>
-    </row>
-    <row r="3414" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3414" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3414" s="1" t="s">
         <v>6</v>
       </c>
@@ -58619,7 +58587,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="3415" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3415" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3415" s="1" t="s">
         <v>7</v>
       </c>
@@ -58636,7 +58604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3416" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3416" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3416" s="1" t="s">
         <v>8</v>
       </c>
@@ -58653,7 +58621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3417" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3417" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3417" s="1" t="s">
         <v>9</v>
       </c>
@@ -58670,7 +58638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3418" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3418" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3418" s="1" t="s">
         <v>10</v>
       </c>
@@ -58687,7 +58655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3419" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3419" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3419" s="1" t="s">
         <v>11</v>
       </c>
@@ -58704,7 +58672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3420" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3420" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3420" s="1" t="s">
         <v>12</v>
       </c>
@@ -58721,7 +58689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3421" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3421" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3421" s="1" t="s">
         <v>13</v>
       </c>
@@ -58738,7 +58706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3422" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3422" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3422" s="1" t="s">
         <v>5</v>
       </c>
@@ -58755,7 +58723,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="3423" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3423" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3423" s="1" t="s">
         <v>6</v>
       </c>
@@ -58772,7 +58740,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="3424" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3424" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3424" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>